<commit_message>
Updated for results writing
</commit_message>
<xml_diff>
--- a/figs/SuppTables.xlsx
+++ b/figs/SuppTables.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="900" documentId="8_{F97B7B36-F9D2-4253-8351-EBD5DC27800B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7CD21424-FBD5-4ED6-B4E7-FDC9B69F4341}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="5" xr2:uid="{30FE7BD5-8B58-4EDD-8F6A-E831DA3D3B84}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="1" activeTab="5" xr2:uid="{30FE7BD5-8B58-4EDD-8F6A-E831DA3D3B84}"/>
   </bookViews>
   <sheets>
     <sheet name="Table S1" sheetId="2" r:id="rId1"/>
@@ -913,7 +913,7 @@
   <numFmts count="3">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="0.000"/>
-    <numFmt numFmtId="172" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="10" x14ac:knownFonts="1">
     <font>
@@ -1044,25 +1044,25 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="172" fontId="7" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="172" fontId="7" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="172" fontId="8" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="172" fontId="7" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="8" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="172" fontId="7" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="172" fontId="8" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="8" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="7" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1396,40 +1396,40 @@
       <selection activeCell="A4" sqref="A4:XFD30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="5" customWidth="1"/>
-    <col min="3" max="3" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="4.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="5.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="21.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="19" max="21" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="4.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="21.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="21" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="10.6640625" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="11" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="20.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="3" spans="1:26" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:26" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
         <v>10</v>
       </c>
@@ -1509,7 +1509,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3998</v>
       </c>
@@ -1592,7 +1592,7 @@
         <v>0.12337662337662338</v>
       </c>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>3987</v>
       </c>
@@ -1675,7 +1675,7 @@
         <v>0.15189873417721519</v>
       </c>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>4023</v>
       </c>
@@ -1758,7 +1758,7 @@
         <v>0.15789473684210525</v>
       </c>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>3993</v>
       </c>
@@ -1841,7 +1841,7 @@
         <v>0.13580246913580246</v>
       </c>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>4033</v>
       </c>
@@ -1924,7 +1924,7 @@
         <v>0.1524390243902439</v>
       </c>
     </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>3985</v>
       </c>
@@ -2007,7 +2007,7 @@
         <v>0.13333333333333333</v>
       </c>
     </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>3999</v>
       </c>
@@ -2090,7 +2090,7 @@
         <v>0.17261904761904762</v>
       </c>
     </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>3990</v>
       </c>
@@ -2173,7 +2173,7 @@
         <v>0.1893491124260355</v>
       </c>
     </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>4012</v>
       </c>
@@ -2256,7 +2256,7 @@
         <v>0.13294797687861271</v>
       </c>
     </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>4025</v>
       </c>
@@ -2339,7 +2339,7 @@
         <v>0.11494252873563218</v>
       </c>
     </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>4046</v>
       </c>
@@ -2422,7 +2422,7 @@
         <v>0.14367816091954022</v>
       </c>
     </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>4119</v>
       </c>
@@ -2503,7 +2503,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>4130</v>
       </c>
@@ -2584,7 +2584,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="17" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>4128</v>
       </c>
@@ -2665,7 +2665,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="18" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>4108</v>
       </c>
@@ -2746,7 +2746,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="19" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>4150</v>
       </c>
@@ -2827,7 +2827,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="20" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>4085</v>
       </c>
@@ -2908,7 +2908,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="21" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>4127</v>
       </c>
@@ -2989,7 +2989,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="22" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>4090</v>
       </c>
@@ -3070,7 +3070,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="23" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>4116</v>
       </c>
@@ -3151,7 +3151,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="24" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>4095</v>
       </c>
@@ -3232,7 +3232,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="25" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>4155</v>
       </c>
@@ -3313,7 +3313,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="26" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>4110</v>
       </c>
@@ -3394,7 +3394,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="27" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>4118</v>
       </c>
@@ -3475,7 +3475,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="28" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>4167</v>
       </c>
@@ -3556,7 +3556,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="29" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>4146</v>
       </c>
@@ -3637,7 +3637,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="30" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>4098</v>
       </c>
@@ -3718,7 +3718,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="31" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>3964</v>
       </c>
@@ -3798,7 +3798,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="32" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>3981</v>
       </c>
@@ -3878,7 +3878,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="33" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>4022</v>
       </c>
@@ -3958,7 +3958,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="34" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>3991</v>
       </c>
@@ -4038,7 +4038,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="35" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>4016</v>
       </c>
@@ -4118,7 +4118,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="36" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>4029</v>
       </c>
@@ -4198,7 +4198,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="37" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>3992</v>
       </c>
@@ -4278,7 +4278,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="38" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>4026</v>
       </c>
@@ -4358,7 +4358,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="39" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>3967</v>
       </c>
@@ -4438,7 +4438,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="40" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>4045</v>
       </c>
@@ -4518,7 +4518,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="41" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>4002</v>
       </c>
@@ -4598,7 +4598,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="42" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>4043</v>
       </c>
@@ -4678,7 +4678,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="43" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>4000</v>
       </c>
@@ -4758,7 +4758,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="44" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>4010</v>
       </c>
@@ -4838,7 +4838,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="45" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>4038</v>
       </c>
@@ -4918,7 +4918,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="46" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>4036</v>
       </c>
@@ -4998,7 +4998,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="47" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>4007</v>
       </c>
@@ -5078,7 +5078,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="48" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>3982</v>
       </c>
@@ -5158,7 +5158,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="49" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>4019</v>
       </c>
@@ -5238,7 +5238,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="50" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>4126</v>
       </c>
@@ -5318,7 +5318,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="51" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>4142</v>
       </c>
@@ -5398,7 +5398,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="52" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>4134</v>
       </c>
@@ -5478,7 +5478,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="53" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>4154</v>
       </c>
@@ -5558,7 +5558,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="54" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>4081</v>
       </c>
@@ -5638,7 +5638,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="55" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>4097</v>
       </c>
@@ -5718,7 +5718,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="56" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>4089</v>
       </c>
@@ -5798,7 +5798,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="57" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>4143</v>
       </c>
@@ -5878,7 +5878,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="58" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>4169</v>
       </c>
@@ -5958,7 +5958,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="59" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>4106</v>
       </c>
@@ -6038,7 +6038,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="60" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>4013</v>
       </c>
@@ -6121,7 +6121,7 @@
         <v>0.14035087719298245</v>
       </c>
     </row>
-    <row r="61" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>4056</v>
       </c>
@@ -6204,7 +6204,7 @@
         <v>0.12295081967213115</v>
       </c>
     </row>
-    <row r="62" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>4040</v>
       </c>
@@ -6287,7 +6287,7 @@
         <v>0.18018018018018017</v>
       </c>
     </row>
-    <row r="63" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>3986</v>
       </c>
@@ -6370,7 +6370,7 @@
         <v>0.14754098360655737</v>
       </c>
     </row>
-    <row r="64" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>4028</v>
       </c>
@@ -6453,7 +6453,7 @@
         <v>0.11504424778761062</v>
       </c>
     </row>
-    <row r="65" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>4006</v>
       </c>
@@ -6536,7 +6536,7 @@
         <v>0.13636363636363635</v>
       </c>
     </row>
-    <row r="66" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>4042</v>
       </c>
@@ -6619,7 +6619,7 @@
         <v>0.16260162601626016</v>
       </c>
     </row>
-    <row r="67" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>4035</v>
       </c>
@@ -6702,7 +6702,7 @@
         <v>0.11450381679389313</v>
       </c>
     </row>
-    <row r="68" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A68">
         <v>4048</v>
       </c>
@@ -6785,7 +6785,7 @@
         <v>0.16521739130434782</v>
       </c>
     </row>
-    <row r="69" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>3997</v>
       </c>
@@ -6868,7 +6868,7 @@
         <v>0.15217391304347827</v>
       </c>
     </row>
-    <row r="70" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A70">
         <v>4011</v>
       </c>
@@ -6951,7 +6951,7 @@
         <v>9.1603053435114504E-2</v>
       </c>
     </row>
-    <row r="71" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A71">
         <v>3970</v>
       </c>
@@ -7034,7 +7034,7 @@
         <v>0.13970588235294118</v>
       </c>
     </row>
-    <row r="72" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A72">
         <v>3976</v>
       </c>
@@ -7117,7 +7117,7 @@
         <v>0.15454545454545454</v>
       </c>
     </row>
-    <row r="73" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A73">
         <v>4054</v>
       </c>
@@ -7200,7 +7200,7 @@
         <v>0.13385826771653545</v>
       </c>
     </row>
-    <row r="74" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A74">
         <v>3989</v>
       </c>
@@ -7283,7 +7283,7 @@
         <v>0.12598425196850394</v>
       </c>
     </row>
-    <row r="75" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A75">
         <v>4050</v>
       </c>
@@ -7366,7 +7366,7 @@
         <v>0.14285714285714285</v>
       </c>
     </row>
-    <row r="76" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A76">
         <v>3975</v>
       </c>
@@ -7449,7 +7449,7 @@
         <v>0.14492753623188406</v>
       </c>
     </row>
-    <row r="77" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A77">
         <v>4014</v>
       </c>
@@ -7532,7 +7532,7 @@
         <v>0.12949640287769784</v>
       </c>
     </row>
-    <row r="78" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A78">
         <v>4017</v>
       </c>
@@ -7615,7 +7615,7 @@
         <v>0.14583333333333334</v>
       </c>
     </row>
-    <row r="79" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A79">
         <v>4004</v>
       </c>
@@ -7698,7 +7698,7 @@
         <v>0.13194444444444445</v>
       </c>
     </row>
-    <row r="80" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A80">
         <v>4152</v>
       </c>
@@ -7779,7 +7779,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="81" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A81">
         <v>4161</v>
       </c>
@@ -7860,7 +7860,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="82" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A82">
         <v>4172</v>
       </c>
@@ -7941,7 +7941,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="83" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A83">
         <v>4173</v>
       </c>
@@ -8022,7 +8022,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="84" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A84">
         <v>4188</v>
       </c>
@@ -8103,7 +8103,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="85" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A85">
         <v>4117</v>
       </c>
@@ -8184,7 +8184,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="86" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A86">
         <v>4148</v>
       </c>
@@ -8265,7 +8265,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="87" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A87">
         <v>4115</v>
       </c>
@@ -8359,15 +8359,15 @@
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.42578125" customWidth="1"/>
-    <col min="2" max="2" width="33.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.44140625" customWidth="1"/>
+    <col min="2" max="2" width="33.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>169</v>
       </c>
@@ -8375,7 +8375,7 @@
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>170</v>
       </c>
@@ -8389,7 +8389,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>171</v>
       </c>
@@ -8403,7 +8403,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>5</v>
       </c>
@@ -8414,7 +8414,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
         <v>6</v>
       </c>
@@ -8425,7 +8425,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
         <v>7</v>
       </c>
@@ -8449,9 +8449,9 @@
       <selection activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>168</v>
       </c>
@@ -8469,29 +8469,29 @@
       <selection activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="32.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="32.109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="28" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="36.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="26.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="39.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="40.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="41.28515625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="22.28515625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="36.88671875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="26.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="39.44140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="40.44140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="41.33203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="20.33203125" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="20" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="21.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>167</v>
       </c>
@@ -8510,33 +8510,33 @@
       <selection pane="topRight" activeCell="K36" sqref="K36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.28515625" customWidth="1"/>
-    <col min="2" max="3" width="20.140625" customWidth="1"/>
-    <col min="4" max="4" width="29.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="29.140625" customWidth="1"/>
-    <col min="6" max="6" width="26.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.33203125" customWidth="1"/>
+    <col min="2" max="3" width="20.109375" customWidth="1"/>
+    <col min="4" max="4" width="29.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="29.109375" customWidth="1"/>
+    <col min="6" max="6" width="26.5546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="36" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="24.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="38.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="39.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="24.88671875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="38.5546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.88671875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="39.88671875" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="41" customWidth="1"/>
-    <col min="14" max="14" width="22.28515625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="18.5703125" customWidth="1"/>
-    <col min="17" max="17" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="18.5546875" customWidth="1"/>
+    <col min="17" max="17" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="21.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="3" spans="1:18" s="18" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="21" t="s">
         <v>130</v>
       </c>
@@ -8592,7 +8592,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="4" spans="1:18" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" s="16" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="16" t="s">
         <v>147</v>
       </c>
@@ -8600,14 +8600,14 @@
         <v>46838072</v>
       </c>
       <c r="C4" s="19">
-        <f>B4*2</f>
+        <f t="shared" ref="C4:C19" si="0">B4*2</f>
         <v>93676144</v>
       </c>
       <c r="D4" s="16">
         <v>86411796</v>
       </c>
       <c r="E4" s="16">
-        <f>D4/2</f>
+        <f t="shared" ref="E4:E19" si="1">D4/2</f>
         <v>43205898</v>
       </c>
       <c r="F4" s="16">
@@ -8650,7 +8650,7 @@
         <v>76979</v>
       </c>
     </row>
-    <row r="5" spans="1:18" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" s="16" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="16" t="s">
         <v>149</v>
       </c>
@@ -8658,14 +8658,14 @@
         <v>42276614</v>
       </c>
       <c r="C5" s="19">
-        <f>B5*2</f>
+        <f t="shared" si="0"/>
         <v>84553228</v>
       </c>
       <c r="D5" s="16">
         <v>76362876</v>
       </c>
       <c r="E5" s="16">
-        <f>D5/2</f>
+        <f t="shared" si="1"/>
         <v>38181438</v>
       </c>
       <c r="F5" s="16">
@@ -8708,7 +8708,7 @@
         <v>56609</v>
       </c>
     </row>
-    <row r="6" spans="1:18" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" s="16" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="16" t="s">
         <v>151</v>
       </c>
@@ -8716,14 +8716,14 @@
         <v>25732843</v>
       </c>
       <c r="C6" s="19">
-        <f>B6*2</f>
+        <f t="shared" si="0"/>
         <v>51465686</v>
       </c>
       <c r="D6" s="16">
         <v>45674864</v>
       </c>
       <c r="E6" s="16">
-        <f>D6/2</f>
+        <f t="shared" si="1"/>
         <v>22837432</v>
       </c>
       <c r="F6" s="16">
@@ -8766,7 +8766,7 @@
         <v>47957</v>
       </c>
     </row>
-    <row r="7" spans="1:18" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" s="16" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="16" t="s">
         <v>137</v>
       </c>
@@ -8774,14 +8774,14 @@
         <v>44652161</v>
       </c>
       <c r="C7" s="19">
-        <f>B7*2</f>
+        <f t="shared" si="0"/>
         <v>89304322</v>
       </c>
       <c r="D7" s="16">
         <v>84170856</v>
       </c>
       <c r="E7" s="16">
-        <f>D7/2</f>
+        <f t="shared" si="1"/>
         <v>42085428</v>
       </c>
       <c r="F7" s="16">
@@ -8824,7 +8824,7 @@
         <v>77302</v>
       </c>
     </row>
-    <row r="8" spans="1:18" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:18" s="16" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="16" t="s">
         <v>139</v>
       </c>
@@ -8832,14 +8832,14 @@
         <v>66266524</v>
       </c>
       <c r="C8" s="19">
-        <f>B8*2</f>
+        <f t="shared" si="0"/>
         <v>132533048</v>
       </c>
       <c r="D8" s="16">
         <v>118150456</v>
       </c>
       <c r="E8" s="16">
-        <f>D8/2</f>
+        <f t="shared" si="1"/>
         <v>59075228</v>
       </c>
       <c r="F8" s="16">
@@ -8882,7 +8882,7 @@
         <v>68146</v>
       </c>
     </row>
-    <row r="9" spans="1:18" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:18" s="16" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="16" t="s">
         <v>141</v>
       </c>
@@ -8890,14 +8890,14 @@
         <v>47317657</v>
       </c>
       <c r="C9" s="19">
-        <f>B9*2</f>
+        <f t="shared" si="0"/>
         <v>94635314</v>
       </c>
       <c r="D9" s="16">
         <v>85309948</v>
       </c>
       <c r="E9" s="16">
-        <f>D9/2</f>
+        <f t="shared" si="1"/>
         <v>42654974</v>
       </c>
       <c r="F9" s="16">
@@ -8940,7 +8940,7 @@
         <v>56877</v>
       </c>
     </row>
-    <row r="10" spans="1:18" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:18" s="16" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="16" t="s">
         <v>142</v>
       </c>
@@ -8948,14 +8948,14 @@
         <v>32448462</v>
       </c>
       <c r="C10" s="19">
-        <f>B10*2</f>
+        <f t="shared" si="0"/>
         <v>64896924</v>
       </c>
       <c r="D10" s="16">
         <v>54400122</v>
       </c>
       <c r="E10" s="16">
-        <f>D10/2</f>
+        <f t="shared" si="1"/>
         <v>27200061</v>
       </c>
       <c r="F10" s="16">
@@ -8998,7 +8998,7 @@
         <v>42341</v>
       </c>
     </row>
-    <row r="11" spans="1:18" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18" s="16" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A11" s="16" t="s">
         <v>143</v>
       </c>
@@ -9006,14 +9006,14 @@
         <v>35265844</v>
       </c>
       <c r="C11" s="19">
-        <f>B11*2</f>
+        <f t="shared" si="0"/>
         <v>70531688</v>
       </c>
       <c r="D11" s="16">
         <v>64894874</v>
       </c>
       <c r="E11" s="16">
-        <f>D11/2</f>
+        <f t="shared" si="1"/>
         <v>32447437</v>
       </c>
       <c r="F11" s="16">
@@ -9056,7 +9056,7 @@
         <v>40442</v>
       </c>
     </row>
-    <row r="12" spans="1:18" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:18" s="16" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A12" s="16" t="s">
         <v>144</v>
       </c>
@@ -9064,14 +9064,14 @@
         <v>37486950</v>
       </c>
       <c r="C12" s="19">
-        <f>B12*2</f>
+        <f t="shared" si="0"/>
         <v>74973900</v>
       </c>
       <c r="D12" s="16">
         <v>70166674</v>
       </c>
       <c r="E12" s="16">
-        <f>D12/2</f>
+        <f t="shared" si="1"/>
         <v>35083337</v>
       </c>
       <c r="F12" s="16">
@@ -9114,7 +9114,7 @@
         <v>50022</v>
       </c>
     </row>
-    <row r="13" spans="1:18" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:18" s="16" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A13" s="16" t="s">
         <v>148</v>
       </c>
@@ -9122,14 +9122,14 @@
         <v>47551808</v>
       </c>
       <c r="C13" s="19">
-        <f>B13*2</f>
+        <f t="shared" si="0"/>
         <v>95103616</v>
       </c>
       <c r="D13" s="16">
         <v>87656018</v>
       </c>
       <c r="E13" s="16">
-        <f>D13/2</f>
+        <f t="shared" si="1"/>
         <v>43828009</v>
       </c>
       <c r="F13" s="17">
@@ -9172,7 +9172,7 @@
         <v>53517</v>
       </c>
     </row>
-    <row r="14" spans="1:18" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:18" s="16" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A14" s="16" t="s">
         <v>150</v>
       </c>
@@ -9180,14 +9180,14 @@
         <v>30894526</v>
       </c>
       <c r="C14" s="19">
-        <f>B14*2</f>
+        <f t="shared" si="0"/>
         <v>61789052</v>
       </c>
       <c r="D14" s="16">
         <v>57204632</v>
       </c>
       <c r="E14" s="16">
-        <f>D14/2</f>
+        <f t="shared" si="1"/>
         <v>28602316</v>
       </c>
       <c r="F14" s="17">
@@ -9230,7 +9230,7 @@
         <v>55925</v>
       </c>
     </row>
-    <row r="15" spans="1:18" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:18" s="16" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A15" s="16" t="s">
         <v>152</v>
       </c>
@@ -9238,14 +9238,14 @@
         <v>36595994</v>
       </c>
       <c r="C15" s="19">
-        <f>B15*2</f>
+        <f t="shared" si="0"/>
         <v>73191988</v>
       </c>
       <c r="D15" s="16">
         <v>66468650</v>
       </c>
       <c r="E15" s="16">
-        <f>D15/2</f>
+        <f t="shared" si="1"/>
         <v>33234325</v>
       </c>
       <c r="F15" s="17">
@@ -9288,7 +9288,7 @@
         <v>65682</v>
       </c>
     </row>
-    <row r="16" spans="1:18" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:18" s="16" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A16" s="16" t="s">
         <v>136</v>
       </c>
@@ -9296,14 +9296,14 @@
         <v>67016346</v>
       </c>
       <c r="C16" s="19">
-        <f>B16*2</f>
+        <f t="shared" si="0"/>
         <v>134032692</v>
       </c>
       <c r="D16" s="16">
         <v>125178902</v>
       </c>
       <c r="E16" s="16">
-        <f>D16/2</f>
+        <f t="shared" si="1"/>
         <v>62589451</v>
       </c>
       <c r="F16" s="17">
@@ -9346,7 +9346,7 @@
         <v>108601</v>
       </c>
     </row>
-    <row r="17" spans="1:18" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:18" s="16" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A17" s="16" t="s">
         <v>138</v>
       </c>
@@ -9354,14 +9354,14 @@
         <v>26529822</v>
       </c>
       <c r="C17" s="19">
-        <f>B17*2</f>
+        <f t="shared" si="0"/>
         <v>53059644</v>
       </c>
       <c r="D17" s="16">
         <v>47747300</v>
       </c>
       <c r="E17" s="16">
-        <f>D17/2</f>
+        <f t="shared" si="1"/>
         <v>23873650</v>
       </c>
       <c r="F17" s="17">
@@ -9404,7 +9404,7 @@
         <v>51233</v>
       </c>
     </row>
-    <row r="18" spans="1:18" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:18" s="16" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A18" s="16" t="s">
         <v>140</v>
       </c>
@@ -9412,14 +9412,14 @@
         <v>40390944</v>
       </c>
       <c r="C18" s="19">
-        <f>B18*2</f>
+        <f t="shared" si="0"/>
         <v>80781888</v>
       </c>
       <c r="D18" s="16">
         <v>74574878</v>
       </c>
       <c r="E18" s="16">
-        <f>D18/2</f>
+        <f t="shared" si="1"/>
         <v>37287439</v>
       </c>
       <c r="F18" s="17">
@@ -9462,7 +9462,7 @@
         <v>43891</v>
       </c>
     </row>
-    <row r="19" spans="1:18" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:18" s="16" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A19" s="16" t="s">
         <v>165</v>
       </c>
@@ -9470,14 +9470,14 @@
         <v>35342939</v>
       </c>
       <c r="C19" s="19">
-        <f>B19*2</f>
+        <f t="shared" si="0"/>
         <v>70685878</v>
       </c>
       <c r="D19" s="16">
         <v>63998016</v>
       </c>
       <c r="E19" s="16">
-        <f>D19/2</f>
+        <f t="shared" si="1"/>
         <v>31999008</v>
       </c>
       <c r="F19" s="17">
@@ -9520,7 +9520,7 @@
         <v>22914</v>
       </c>
     </row>
-    <row r="20" spans="1:18" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:18" s="16" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A20" s="16" t="s">
         <v>145</v>
       </c>
@@ -9528,14 +9528,14 @@
         <v>38274685</v>
       </c>
       <c r="C20" s="19">
-        <f t="shared" ref="C20:C21" si="0">B20*2</f>
+        <f t="shared" ref="C20:C21" si="2">B20*2</f>
         <v>76549370</v>
       </c>
       <c r="D20" s="16">
         <v>62269198</v>
       </c>
       <c r="E20" s="16">
-        <f t="shared" ref="E20:E21" si="1">D20/2</f>
+        <f t="shared" ref="E20:E21" si="3">D20/2</f>
         <v>31134599</v>
       </c>
       <c r="F20" s="17">
@@ -9578,7 +9578,7 @@
         <v>46857</v>
       </c>
     </row>
-    <row r="21" spans="1:18" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:18" s="16" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A21" s="16" t="s">
         <v>146</v>
       </c>
@@ -9586,14 +9586,14 @@
         <v>33144427</v>
       </c>
       <c r="C21" s="19">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>66288854</v>
       </c>
       <c r="D21" s="16">
         <v>57277596</v>
       </c>
       <c r="E21" s="16">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>28638798</v>
       </c>
       <c r="F21" s="17">
@@ -9636,147 +9636,147 @@
         <v>36555</v>
       </c>
     </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B23" s="24">
-        <f>AVERAGE(B4:B21)</f>
+        <f t="shared" ref="B23:R23" si="4">AVERAGE(B4:B21)</f>
         <v>40779256.555555552</v>
       </c>
       <c r="C23" s="24">
-        <f>AVERAGE(C4:C21)</f>
+        <f t="shared" si="4"/>
         <v>81558513.111111104</v>
       </c>
       <c r="D23" s="24">
-        <f>AVERAGE(D4:D21)</f>
+        <f t="shared" si="4"/>
         <v>73773203.111111104</v>
       </c>
       <c r="E23" s="24">
-        <f>AVERAGE(E4:E21)</f>
+        <f t="shared" si="4"/>
         <v>36886601.555555552</v>
       </c>
       <c r="F23" s="24">
-        <f>AVERAGE(F4:F21)</f>
+        <f t="shared" si="4"/>
         <v>534751</v>
       </c>
       <c r="G23" s="24">
-        <f>AVERAGE(G4:G21)</f>
+        <f t="shared" si="4"/>
         <v>75028.166666666672</v>
       </c>
       <c r="H23" s="24">
-        <f>AVERAGE(H4:H21)</f>
+        <f t="shared" si="4"/>
         <v>504613961.8888889</v>
       </c>
       <c r="I23" s="24">
-        <f>AVERAGE(I4:I21)</f>
+        <f t="shared" si="4"/>
         <v>302198261.44444442</v>
       </c>
       <c r="J23" s="24">
-        <f>AVERAGE(J4:J21)</f>
+        <f t="shared" si="4"/>
         <v>2704.3333333333335</v>
       </c>
       <c r="K23" s="24">
-        <f>AVERAGE(K4:K21)</f>
+        <f t="shared" si="4"/>
         <v>31627.5</v>
       </c>
       <c r="L23" s="24">
-        <f>AVERAGE(L4:L21)</f>
+        <f t="shared" si="4"/>
         <v>4.3300000000000018</v>
       </c>
       <c r="M23" s="24">
-        <f>AVERAGE(M4:M21)</f>
+        <f t="shared" si="4"/>
         <v>95.581666666666649</v>
       </c>
       <c r="N23" s="24">
-        <f>AVERAGE(N4:N21)</f>
+        <f t="shared" si="4"/>
         <v>3357466.0947011379</v>
       </c>
       <c r="O23" s="24">
-        <f>AVERAGE(O4:O21)</f>
+        <f t="shared" si="4"/>
         <v>3288.738772515509</v>
       </c>
       <c r="P23" s="24">
-        <f>AVERAGE(P4:P21)</f>
+        <f t="shared" si="4"/>
         <v>0.40612366872222228</v>
       </c>
       <c r="Q23" s="24">
-        <f>AVERAGE(Q4:Q21)</f>
+        <f t="shared" si="4"/>
         <v>849817.61111111112</v>
       </c>
       <c r="R23" s="24">
-        <f>AVERAGE(R4:R21)</f>
+        <f t="shared" si="4"/>
         <v>55658.333333333336</v>
       </c>
     </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B24">
-        <f>STDEV(B4:B21)</f>
+        <f t="shared" ref="B24:R24" si="5">STDEV(B4:B21)</f>
         <v>11453512.214728422</v>
       </c>
       <c r="C24">
-        <f>STDEV(C4:C21)</f>
+        <f t="shared" si="5"/>
         <v>22907024.429456845</v>
       </c>
       <c r="D24">
-        <f>STDEV(D4:D21)</f>
+        <f t="shared" si="5"/>
         <v>21658849.09352934</v>
       </c>
       <c r="E24">
-        <f>STDEV(E4:E21)</f>
+        <f t="shared" si="5"/>
         <v>10829424.54676467</v>
       </c>
       <c r="F24">
-        <f>STDEV(F4:F21)</f>
+        <f t="shared" si="5"/>
         <v>222450.26675615014</v>
       </c>
       <c r="G24">
-        <f>STDEV(G4:G21)</f>
+        <f t="shared" si="5"/>
         <v>28445.917948130358</v>
       </c>
       <c r="H24">
-        <f>STDEV(H4:H21)</f>
+        <f t="shared" si="5"/>
         <v>176769005.99747348</v>
       </c>
       <c r="I24">
-        <f>STDEV(I4:I21)</f>
+        <f t="shared" si="5"/>
         <v>125289676.15453173</v>
       </c>
       <c r="J24">
-        <f>STDEV(J4:J21)</f>
+        <f t="shared" si="5"/>
         <v>1793.1551227146097</v>
       </c>
       <c r="K24">
-        <f>STDEV(K4:K21)</f>
+        <f t="shared" si="5"/>
         <v>20204.921215474449</v>
       </c>
       <c r="L24">
-        <f>STDEV(L4:L21)</f>
+        <f t="shared" si="5"/>
         <v>3.4306524846723003</v>
       </c>
       <c r="M24">
-        <f>STDEV(M4:M21)</f>
+        <f t="shared" si="5"/>
         <v>1.4029894553291211</v>
       </c>
       <c r="N24">
-        <f>STDEV(N4:N21)</f>
+        <f t="shared" si="5"/>
         <v>389707.71736475412</v>
       </c>
       <c r="O24">
-        <f>STDEV(O4:O21)</f>
+        <f t="shared" si="5"/>
         <v>976.24581368288091</v>
       </c>
       <c r="P24">
-        <f>STDEV(P4:P21)</f>
+        <f t="shared" si="5"/>
         <v>0.3530879603985258</v>
       </c>
       <c r="Q24">
-        <f>STDEV(Q4:Q21)</f>
+        <f t="shared" si="5"/>
         <v>326127.86135973589</v>
       </c>
       <c r="R24">
-        <f>STDEV(R4:R21)</f>
+        <f t="shared" si="5"/>
         <v>19038.689676241778</v>
       </c>
     </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B25">
         <f>B24/SQRT(18)</f>
         <v>2699618.7184791402</v>
@@ -9786,23 +9786,23 @@
         <v>5399237.4369582804</v>
       </c>
       <c r="D25">
-        <f t="shared" ref="D25:H25" si="2">D24/SQRT(18)</f>
+        <f t="shared" ref="D25:H25" si="6">D24/SQRT(18)</f>
         <v>5105039.6889102347</v>
       </c>
       <c r="E25">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>2552519.8444551174</v>
       </c>
       <c r="F25">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>52432.030700010066</v>
       </c>
       <c r="G25">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>6704.7671593997002</v>
       </c>
       <c r="H25">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>41664854.281472996</v>
       </c>
       <c r="I25">
@@ -9810,183 +9810,183 @@
         <v>30387209.916739095</v>
       </c>
       <c r="J25">
-        <f t="shared" ref="J25:R25" si="3">J24/SQRT(17)</f>
+        <f t="shared" ref="J25:R25" si="7">J24/SQRT(17)</f>
         <v>434.90399847469018</v>
       </c>
       <c r="K25">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>4900.4131958049602</v>
       </c>
       <c r="L25">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>0.83205544465244508</v>
       </c>
       <c r="M25">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>0.34027492446763274</v>
       </c>
       <c r="N25">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>94518.004812543237</v>
       </c>
       <c r="O25">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>236.77438861068097</v>
       </c>
       <c r="P25">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>8.5636409168060437E-2</v>
       </c>
       <c r="Q25">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>79097.624696646089</v>
       </c>
       <c r="R25">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>4617.5605005000798</v>
       </c>
     </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B26" s="24">
-        <f>MIN(B4:B21)</f>
+        <f t="shared" ref="B26:R26" si="8">MIN(B4:B21)</f>
         <v>25732843</v>
       </c>
       <c r="C26" s="24">
-        <f>MIN(C4:C21)</f>
+        <f t="shared" si="8"/>
         <v>51465686</v>
       </c>
       <c r="D26" s="24">
-        <f>MIN(D4:D21)</f>
+        <f t="shared" si="8"/>
         <v>45674864</v>
       </c>
       <c r="E26" s="24">
-        <f>MIN(E4:E21)</f>
+        <f t="shared" si="8"/>
         <v>22837432</v>
       </c>
       <c r="F26" s="24">
-        <f>MIN(F4:F21)</f>
+        <f t="shared" si="8"/>
         <v>170433</v>
       </c>
       <c r="G26" s="24">
-        <f>MIN(G4:G21)</f>
+        <f t="shared" si="8"/>
         <v>22668</v>
       </c>
       <c r="H26" s="24">
-        <f>MIN(H4:H21)</f>
+        <f t="shared" si="8"/>
         <v>206778444</v>
       </c>
       <c r="I26" s="24">
-        <f>MIN(I4:I21)</f>
+        <f t="shared" si="8"/>
         <v>28953925</v>
       </c>
       <c r="J26" s="24">
-        <f>MIN(J4:J21)</f>
+        <f t="shared" si="8"/>
         <v>1274</v>
       </c>
       <c r="K26" s="24">
-        <f>MIN(K4:K21)</f>
+        <f t="shared" si="8"/>
         <v>2903</v>
       </c>
       <c r="L26" s="24">
-        <f>MIN(L4:L21)</f>
+        <f t="shared" si="8"/>
         <v>1.41</v>
       </c>
       <c r="M26" s="24">
-        <f>MIN(M4:M21)</f>
+        <f t="shared" si="8"/>
         <v>92.92</v>
       </c>
       <c r="N26" s="24">
-        <f>MIN(N4:N21)</f>
+        <f t="shared" si="8"/>
         <v>2693300.7037427099</v>
       </c>
       <c r="O26" s="24">
-        <f>MIN(O4:O21)</f>
+        <f t="shared" si="8"/>
         <v>1931.2579208053801</v>
       </c>
       <c r="P26" s="24">
-        <f>MIN(P4:P21)</f>
+        <f t="shared" si="8"/>
         <v>8.0178515000000006E-2</v>
       </c>
       <c r="Q26" s="24">
-        <f>MIN(Q4:Q21)</f>
+        <f t="shared" si="8"/>
         <v>309036</v>
       </c>
       <c r="R26" s="24">
-        <f>MIN(R4:R21)</f>
+        <f t="shared" si="8"/>
         <v>22914</v>
       </c>
     </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B27" s="24">
-        <f>MAX(B4:B21)</f>
+        <f t="shared" ref="B27:R27" si="9">MAX(B4:B21)</f>
         <v>67016346</v>
       </c>
       <c r="C27" s="24">
-        <f>MAX(C4:C21)</f>
+        <f t="shared" si="9"/>
         <v>134032692</v>
       </c>
       <c r="D27" s="24">
-        <f>MAX(D4:D21)</f>
+        <f t="shared" si="9"/>
         <v>125178902</v>
       </c>
       <c r="E27" s="24">
-        <f>MAX(E4:E21)</f>
+        <f t="shared" si="9"/>
         <v>62589451</v>
       </c>
       <c r="F27" s="24">
-        <f>MAX(F4:F21)</f>
+        <f t="shared" si="9"/>
         <v>1039489</v>
       </c>
       <c r="G27" s="24">
-        <f>MAX(G4:G21)</f>
+        <f t="shared" si="9"/>
         <v>140051</v>
       </c>
       <c r="H27" s="24">
-        <f>MAX(H4:H21)</f>
+        <f t="shared" si="9"/>
         <v>940079559</v>
       </c>
       <c r="I27" s="24">
-        <f>MAX(I4:I21)</f>
+        <f t="shared" si="9"/>
         <v>575630547</v>
       </c>
       <c r="J27" s="24">
-        <f>MAX(J4:J21)</f>
+        <f t="shared" si="9"/>
         <v>7725</v>
       </c>
       <c r="K27" s="24">
-        <f>MAX(K4:K21)</f>
+        <f t="shared" si="9"/>
         <v>70788</v>
       </c>
       <c r="L27" s="24">
-        <f>MAX(L4:L21)</f>
+        <f t="shared" si="9"/>
         <v>14.71</v>
       </c>
       <c r="M27" s="24">
-        <f>MAX(M4:M21)</f>
+        <f t="shared" si="9"/>
         <v>97.9</v>
       </c>
       <c r="N27" s="24">
-        <f>MAX(N4:N21)</f>
+        <f t="shared" si="9"/>
         <v>4173023.8708614102</v>
       </c>
       <c r="O27" s="24">
-        <f>MAX(O4:O21)</f>
+        <f t="shared" si="9"/>
         <v>5547.2423780958497</v>
       </c>
       <c r="P27" s="24">
-        <f>MAX(P4:P21)</f>
+        <f t="shared" si="9"/>
         <v>1.680544456</v>
       </c>
       <c r="Q27" s="24">
-        <f>MAX(Q4:Q21)</f>
+        <f t="shared" si="9"/>
         <v>1650758</v>
       </c>
       <c r="R27" s="24">
-        <f>MAX(R4:R21)</f>
+        <f t="shared" si="9"/>
         <v>108601</v>
       </c>
     </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B29" s="24">
         <f>SUM(B4:B21)</f>
         <v>734026618</v>
@@ -10006,27 +10006,27 @@
       <selection activeCell="B69" activeCellId="8" sqref="B40 B42 B45:B46 B50 B52:B56 B58:B59 B64 B66:B67 B69:B70"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="40.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="40.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="6" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.33203125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="13" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="2" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="3" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="4" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="4" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="35" t="s">
         <v>172</v>
       </c>
@@ -10055,7 +10055,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="5" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="13" t="s">
         <v>177</v>
       </c>
@@ -10084,7 +10084,7 @@
         <v>6.3549208439999996</v>
       </c>
     </row>
-    <row r="6" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="29"/>
       <c r="B6" s="29" t="s">
         <v>179</v>
@@ -10111,7 +10111,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="13" t="s">
         <v>180</v>
       </c>
@@ -10140,7 +10140,7 @@
         <v>6.3713679650000001</v>
       </c>
     </row>
-    <row r="8" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B8" s="13" t="s">
         <v>182</v>
       </c>
@@ -10166,7 +10166,7 @@
         <v>0.10879570199999999</v>
       </c>
     </row>
-    <row r="9" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B9" s="13" t="s">
         <v>183</v>
       </c>
@@ -10192,7 +10192,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B10" s="13" t="s">
         <v>184</v>
       </c>
@@ -10218,7 +10218,7 @@
         <v>1.9880800000000001E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B11" s="13" t="s">
         <v>185</v>
       </c>
@@ -10244,7 +10244,7 @@
         <v>7.4184000000000003E-3</v>
       </c>
     </row>
-    <row r="12" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A12" s="29"/>
       <c r="B12" s="29" t="s">
         <v>186</v>
@@ -10271,7 +10271,7 @@
         <v>1.8705409999999999E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A13" s="13" t="s">
         <v>187</v>
       </c>
@@ -10300,7 +10300,7 @@
         <v>6.3588288909999999</v>
       </c>
     </row>
-    <row r="14" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B14" s="27" t="s">
         <v>189</v>
       </c>
@@ -10326,7 +10326,7 @@
         <v>0.10879570199999999</v>
       </c>
     </row>
-    <row r="15" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B15" s="27" t="s">
         <v>190</v>
       </c>
@@ -10352,7 +10352,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B16" s="27" t="s">
         <v>191</v>
       </c>
@@ -10378,7 +10378,7 @@
         <v>6.8306E-3</v>
       </c>
     </row>
-    <row r="17" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B17" s="27" t="s">
         <v>192</v>
       </c>
@@ -10404,7 +10404,7 @@
         <v>1.9880800000000001E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B18" s="27" t="s">
         <v>193</v>
       </c>
@@ -10430,7 +10430,7 @@
         <v>7.4184000000000003E-3</v>
       </c>
     </row>
-    <row r="19" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A19" s="29"/>
       <c r="B19" s="29" t="s">
         <v>194</v>
@@ -10457,7 +10457,7 @@
         <v>1.8257689000000001E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A20" s="13" t="s">
         <v>195</v>
       </c>
@@ -10486,7 +10486,7 @@
         <v>3.057149736</v>
       </c>
     </row>
-    <row r="21" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B21" s="27" t="s">
         <v>198</v>
       </c>
@@ -10512,7 +10512,7 @@
         <v>0.53208760899999996</v>
       </c>
     </row>
-    <row r="22" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B22" s="27" t="s">
         <v>199</v>
       </c>
@@ -10538,7 +10538,7 @@
         <v>0.10879570199999999</v>
       </c>
     </row>
-    <row r="23" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B23" s="27" t="s">
         <v>200</v>
       </c>
@@ -10564,7 +10564,7 @@
         <v>1.5708996999999999E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B24" s="27" t="s">
         <v>201</v>
       </c>
@@ -10590,7 +10590,7 @@
         <v>3.6973616000000001E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B25" s="27" t="s">
         <v>202</v>
       </c>
@@ -10616,7 +10616,7 @@
         <v>6.8306E-3</v>
       </c>
     </row>
-    <row r="26" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B26" s="27" t="s">
         <v>203</v>
       </c>
@@ -10642,7 +10642,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B27" s="27" t="s">
         <v>204</v>
       </c>
@@ -10668,7 +10668,7 @@
         <v>7.4184000000000003E-3</v>
       </c>
     </row>
-    <row r="28" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B28" s="27" t="s">
         <v>205</v>
       </c>
@@ -10694,7 +10694,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A29" s="29"/>
       <c r="B29" s="29" t="s">
         <v>206</v>
@@ -10721,7 +10721,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A30" s="13" t="s">
         <v>207</v>
       </c>
@@ -10750,7 +10750,7 @@
         <v>3.057149736</v>
       </c>
     </row>
-    <row r="31" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B31" s="31" t="s">
         <v>216</v>
       </c>
@@ -10776,7 +10776,7 @@
         <v>0.53686285899999997</v>
       </c>
     </row>
-    <row r="32" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B32" s="31" t="s">
         <v>209</v>
       </c>
@@ -10802,7 +10802,7 @@
         <v>0.10879570199999999</v>
       </c>
     </row>
-    <row r="33" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B33" s="31" t="s">
         <v>210</v>
       </c>
@@ -10828,7 +10828,7 @@
         <v>1.5708996999999999E-2</v>
       </c>
     </row>
-    <row r="34" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B34" s="31" t="s">
         <v>211</v>
       </c>
@@ -10854,7 +10854,7 @@
         <v>1.8226284999999998E-2</v>
       </c>
     </row>
-    <row r="35" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B35" s="31" t="s">
         <v>212</v>
       </c>
@@ -10880,7 +10880,7 @@
         <v>6.8306E-3</v>
       </c>
     </row>
-    <row r="36" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B36" s="31" t="s">
         <v>213</v>
       </c>
@@ -10906,7 +10906,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B37" s="31" t="s">
         <v>215</v>
       </c>
@@ -10932,7 +10932,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A38" s="29"/>
       <c r="B38" s="32" t="s">
         <v>214</v>
@@ -10959,7 +10959,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A39" s="13" t="s">
         <v>217</v>
       </c>
@@ -10988,7 +10988,7 @@
         <v>4.6647821999999999E-2</v>
       </c>
     </row>
-    <row r="40" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B40" s="31" t="s">
         <v>219</v>
       </c>
@@ -11014,7 +11014,7 @@
         <v>0.150891053</v>
       </c>
     </row>
-    <row r="41" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B41" s="31" t="s">
         <v>220</v>
       </c>
@@ -11040,7 +11040,7 @@
         <v>0.52040448100000003</v>
       </c>
     </row>
-    <row r="42" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B42" s="31" t="s">
         <v>221</v>
       </c>
@@ -11066,7 +11066,7 @@
         <v>1.9880800000000001E-2</v>
       </c>
     </row>
-    <row r="43" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B43" s="31" t="s">
         <v>222</v>
       </c>
@@ -11092,7 +11092,7 @@
         <v>2.7251055999999999E-2</v>
       </c>
     </row>
-    <row r="44" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B44" s="31" t="s">
         <v>223</v>
       </c>
@@ -11118,7 +11118,7 @@
         <v>0.241285531</v>
       </c>
     </row>
-    <row r="45" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B45" s="31" t="s">
         <v>224</v>
       </c>
@@ -11144,7 +11144,7 @@
         <v>1.9880800000000001E-2</v>
       </c>
     </row>
-    <row r="46" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B46" s="31" t="s">
         <v>225</v>
       </c>
@@ -11170,7 +11170,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B47" s="31" t="s">
         <v>226</v>
       </c>
@@ -11196,7 +11196,7 @@
         <v>1.328914E-2</v>
       </c>
     </row>
-    <row r="48" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B48" s="31" t="s">
         <v>227</v>
       </c>
@@ -11222,7 +11222,7 @@
         <v>1.328914E-2</v>
       </c>
     </row>
-    <row r="49" spans="2:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:9" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B49" s="31" t="s">
         <v>228</v>
       </c>
@@ -11248,7 +11248,7 @@
         <v>3.6963785999999998E-2</v>
       </c>
     </row>
-    <row r="50" spans="2:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:9" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B50" s="31" t="s">
         <v>229</v>
       </c>
@@ -11274,7 +11274,7 @@
         <v>1.9880800000000001E-2</v>
       </c>
     </row>
-    <row r="51" spans="2:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:9" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B51" s="31" t="s">
         <v>230</v>
       </c>
@@ -11300,7 +11300,7 @@
         <v>8.0589540000000001E-3</v>
       </c>
     </row>
-    <row r="52" spans="2:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:9" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B52" s="31" t="s">
         <v>231</v>
       </c>
@@ -11326,7 +11326,7 @@
         <v>6.8306E-3</v>
       </c>
     </row>
-    <row r="53" spans="2:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:9" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B53" s="31" t="s">
         <v>232</v>
       </c>
@@ -11352,7 +11352,7 @@
         <v>2.5278254E-2</v>
       </c>
     </row>
-    <row r="54" spans="2:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:9" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B54" s="31" t="s">
         <v>233</v>
       </c>
@@ -11378,7 +11378,7 @@
         <v>6.8306E-3</v>
       </c>
     </row>
-    <row r="55" spans="2:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:9" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B55" s="31" t="s">
         <v>234</v>
       </c>
@@ -11404,7 +11404,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="2:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:9" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B56" s="31" t="s">
         <v>235</v>
       </c>
@@ -11430,7 +11430,7 @@
         <v>1.9251471999999999E-2</v>
       </c>
     </row>
-    <row r="57" spans="2:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:9" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B57" s="31" t="s">
         <v>236</v>
       </c>
@@ -11456,7 +11456,7 @@
         <v>1.701040865</v>
       </c>
     </row>
-    <row r="58" spans="2:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:9" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B58" s="31" t="s">
         <v>254</v>
       </c>
@@ -11482,7 +11482,7 @@
         <v>3.9761400000000002E-2</v>
       </c>
     </row>
-    <row r="59" spans="2:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:9" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B59" s="31" t="s">
         <v>237</v>
       </c>
@@ -11508,7 +11508,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="2:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:9" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B60" s="31" t="s">
         <v>238</v>
       </c>
@@ -11534,7 +11534,7 @@
         <v>0.29008224199999999</v>
       </c>
     </row>
-    <row r="61" spans="2:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:9" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B61" s="31" t="s">
         <v>239</v>
       </c>
@@ -11560,7 +11560,7 @@
         <v>2.7639747999999999E-2</v>
       </c>
     </row>
-    <row r="62" spans="2:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:9" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B62" s="31" t="s">
         <v>240</v>
       </c>
@@ -11586,7 +11586,7 @@
         <v>6.4567419000000001E-2</v>
       </c>
     </row>
-    <row r="63" spans="2:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:9" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B63" s="31" t="s">
         <v>241</v>
       </c>
@@ -11612,7 +11612,7 @@
         <v>3.8624200999999997E-2</v>
       </c>
     </row>
-    <row r="64" spans="2:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:9" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B64" s="31" t="s">
         <v>242</v>
       </c>
@@ -11638,7 +11638,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="2:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:9" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B65" s="31" t="s">
         <v>243</v>
       </c>
@@ -11664,7 +11664,7 @@
         <v>0.103152172</v>
       </c>
     </row>
-    <row r="66" spans="2:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:9" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B66" s="31" t="s">
         <v>244</v>
       </c>
@@ -11690,7 +11690,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="2:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:9" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B67" s="31" t="s">
         <v>245</v>
       </c>
@@ -11716,7 +11716,7 @@
         <v>6.8306E-3</v>
       </c>
     </row>
-    <row r="68" spans="2:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:9" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B68" s="31" t="s">
         <v>246</v>
       </c>
@@ -11742,7 +11742,7 @@
         <v>3.9049671000000001E-2</v>
       </c>
     </row>
-    <row r="69" spans="2:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:9" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B69" s="31" t="s">
         <v>247</v>
       </c>
@@ -11768,7 +11768,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="2:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="2:9" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B70" s="31" t="s">
         <v>248</v>
       </c>
@@ -11794,7 +11794,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="2:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="2:9" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B71" s="31" t="s">
         <v>249</v>
       </c>

</xml_diff>